<commit_message>
Limpieza de Codigo y Agregando el archivo Utils
</commit_message>
<xml_diff>
--- a/Data/Procesado/Desempleo_USA_General.xlsx
+++ b/Data/Procesado/Desempleo_USA_General.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N121"/>
+  <dimension ref="A1:O121"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -480,30 +480,35 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
+          <t>Estado</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
           <t>Blanco_Cantidad</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Negro_Cantidad</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Asiatico_Cantidad</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Hispano_Cantidad</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Hombre_Cantidad</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Mujer_Cantidad</t>
         </is>
@@ -534,22 +539,27 @@
       <c r="H2" t="n">
         <v>7.9</v>
       </c>
-      <c r="I2" t="n">
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J2" t="n">
         <v>16882298</v>
       </c>
-      <c r="J2" t="n">
+      <c r="K2" t="n">
         <v>5975821</v>
       </c>
-      <c r="K2" t="n">
+      <c r="L2" t="n">
         <v>1184858</v>
       </c>
-      <c r="L2" t="n">
+      <c r="M2" t="n">
         <v>6398787</v>
       </c>
-      <c r="M2" t="n">
+      <c r="N2" t="n">
         <v>14966969</v>
       </c>
-      <c r="N2" t="n">
+      <c r="O2" t="n">
         <v>12171632</v>
       </c>
     </row>
@@ -578,22 +588,27 @@
       <c r="H3" t="n">
         <v>8</v>
       </c>
-      <c r="I3" t="n">
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J3" t="n">
         <v>17074142</v>
       </c>
-      <c r="J3" t="n">
+      <c r="K3" t="n">
         <v>5830953</v>
       </c>
-      <c r="K3" t="n">
+      <c r="L3" t="n">
         <v>1170582</v>
       </c>
-      <c r="L3" t="n">
+      <c r="M3" t="n">
         <v>6299581</v>
       </c>
-      <c r="M3" t="n">
+      <c r="N3" t="n">
         <v>15113705</v>
       </c>
-      <c r="N3" t="n">
+      <c r="O3" t="n">
         <v>12325704</v>
       </c>
     </row>
@@ -622,22 +637,27 @@
       <c r="H4" t="n">
         <v>8.1</v>
       </c>
-      <c r="I4" t="n">
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J4" t="n">
         <v>17074142</v>
       </c>
-      <c r="J4" t="n">
+      <c r="K4" t="n">
         <v>6084472</v>
       </c>
-      <c r="K4" t="n">
+      <c r="L4" t="n">
         <v>1084930</v>
       </c>
-      <c r="L4" t="n">
+      <c r="M4" t="n">
         <v>6398787</v>
       </c>
-      <c r="M4" t="n">
+      <c r="N4" t="n">
         <v>14966969</v>
       </c>
-      <c r="N4" t="n">
+      <c r="O4" t="n">
         <v>12479775</v>
       </c>
     </row>
@@ -666,22 +686,27 @@
       <c r="H5" t="n">
         <v>8.300000000000001</v>
       </c>
-      <c r="I5" t="n">
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J5" t="n">
         <v>17265987</v>
       </c>
-      <c r="J5" t="n">
+      <c r="K5" t="n">
         <v>6012038</v>
       </c>
-      <c r="K5" t="n">
+      <c r="L5" t="n">
         <v>999278</v>
       </c>
-      <c r="L5" t="n">
+      <c r="M5" t="n">
         <v>6200375</v>
       </c>
-      <c r="M5" t="n">
+      <c r="N5" t="n">
         <v>14966969</v>
       </c>
-      <c r="N5" t="n">
+      <c r="O5" t="n">
         <v>12787917</v>
       </c>
     </row>
@@ -710,22 +735,27 @@
       <c r="H6" t="n">
         <v>8.1</v>
       </c>
-      <c r="I6" t="n">
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J6" t="n">
         <v>16690454</v>
       </c>
-      <c r="J6" t="n">
+      <c r="K6" t="n">
         <v>5613650</v>
       </c>
-      <c r="K6" t="n">
+      <c r="L6" t="n">
         <v>1113481</v>
       </c>
-      <c r="L6" t="n">
+      <c r="M6" t="n">
         <v>5952360</v>
       </c>
-      <c r="M6" t="n">
+      <c r="N6" t="n">
         <v>14233294</v>
       </c>
-      <c r="N6" t="n">
+      <c r="O6" t="n">
         <v>12479775</v>
       </c>
     </row>
@@ -754,22 +784,27 @@
       <c r="H7" t="n">
         <v>7.7</v>
       </c>
-      <c r="I7" t="n">
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J7" t="n">
         <v>16498609</v>
       </c>
-      <c r="J7" t="n">
+      <c r="K7" t="n">
         <v>5504999</v>
       </c>
-      <c r="K7" t="n">
+      <c r="L7" t="n">
         <v>1056379</v>
       </c>
-      <c r="L7" t="n">
+      <c r="M7" t="n">
         <v>6101169</v>
       </c>
-      <c r="M7" t="n">
+      <c r="N7" t="n">
         <v>14233294</v>
       </c>
-      <c r="N7" t="n">
+      <c r="O7" t="n">
         <v>11863490</v>
       </c>
     </row>
@@ -798,22 +833,27 @@
       <c r="H8" t="n">
         <v>7.9</v>
       </c>
-      <c r="I8" t="n">
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J8" t="n">
         <v>16306765</v>
       </c>
-      <c r="J8" t="n">
+      <c r="K8" t="n">
         <v>5649867</v>
       </c>
-      <c r="K8" t="n">
+      <c r="L8" t="n">
         <v>1127756</v>
       </c>
-      <c r="L8" t="n">
+      <c r="M8" t="n">
         <v>6051566</v>
       </c>
-      <c r="M8" t="n">
+      <c r="N8" t="n">
         <v>14086560</v>
       </c>
-      <c r="N8" t="n">
+      <c r="O8" t="n">
         <v>12171632</v>
       </c>
     </row>
@@ -842,22 +882,27 @@
       <c r="H9" t="n">
         <v>8</v>
       </c>
-      <c r="I9" t="n">
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J9" t="n">
         <v>16498609</v>
       </c>
-      <c r="J9" t="n">
+      <c r="K9" t="n">
         <v>5758518</v>
       </c>
-      <c r="K9" t="n">
+      <c r="L9" t="n">
         <v>1042104</v>
       </c>
-      <c r="L9" t="n">
+      <c r="M9" t="n">
         <v>5952360</v>
       </c>
-      <c r="M9" t="n">
+      <c r="N9" t="n">
         <v>14086560</v>
       </c>
-      <c r="N9" t="n">
+      <c r="O9" t="n">
         <v>12325704</v>
       </c>
     </row>
@@ -886,22 +931,27 @@
       <c r="H10" t="n">
         <v>8</v>
       </c>
-      <c r="I10" t="n">
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J10" t="n">
         <v>16498609</v>
       </c>
-      <c r="J10" t="n">
+      <c r="K10" t="n">
         <v>5794736</v>
       </c>
-      <c r="K10" t="n">
+      <c r="L10" t="n">
         <v>942176</v>
       </c>
-      <c r="L10" t="n">
+      <c r="M10" t="n">
         <v>6101169</v>
       </c>
-      <c r="M10" t="n">
+      <c r="N10" t="n">
         <v>14086560</v>
       </c>
-      <c r="N10" t="n">
+      <c r="O10" t="n">
         <v>12325704</v>
       </c>
     </row>
@@ -930,22 +980,27 @@
       <c r="H11" t="n">
         <v>8</v>
       </c>
-      <c r="I11" t="n">
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J11" t="n">
         <v>16498609</v>
       </c>
-      <c r="J11" t="n">
+      <c r="K11" t="n">
         <v>5649867</v>
       </c>
-      <c r="K11" t="n">
+      <c r="L11" t="n">
         <v>1027828</v>
       </c>
-      <c r="L11" t="n">
+      <c r="M11" t="n">
         <v>6101169</v>
       </c>
-      <c r="M11" t="n">
+      <c r="N11" t="n">
         <v>13793090</v>
       </c>
-      <c r="N11" t="n">
+      <c r="O11" t="n">
         <v>12325704</v>
       </c>
     </row>
@@ -974,22 +1029,27 @@
       <c r="H12" t="n">
         <v>8.4</v>
       </c>
-      <c r="I12" t="n">
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J12" t="n">
         <v>17074142</v>
       </c>
-      <c r="J12" t="n">
+      <c r="K12" t="n">
         <v>5867170</v>
       </c>
-      <c r="K12" t="n">
+      <c r="L12" t="n">
         <v>1070655</v>
       </c>
-      <c r="L12" t="n">
+      <c r="M12" t="n">
         <v>6398787</v>
       </c>
-      <c r="M12" t="n">
+      <c r="N12" t="n">
         <v>14526765</v>
       </c>
-      <c r="N12" t="n">
+      <c r="O12" t="n">
         <v>12941989</v>
       </c>
     </row>
@@ -1018,22 +1078,27 @@
       <c r="H13" t="n">
         <v>8</v>
       </c>
-      <c r="I13" t="n">
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J13" t="n">
         <v>16306765</v>
       </c>
-      <c r="J13" t="n">
+      <c r="K13" t="n">
         <v>5613650</v>
       </c>
-      <c r="K13" t="n">
+      <c r="L13" t="n">
         <v>1027828</v>
       </c>
-      <c r="L13" t="n">
+      <c r="M13" t="n">
         <v>6398787</v>
       </c>
-      <c r="M13" t="n">
+      <c r="N13" t="n">
         <v>13793090</v>
       </c>
-      <c r="N13" t="n">
+      <c r="O13" t="n">
         <v>12325704</v>
       </c>
     </row>
@@ -1062,22 +1127,27 @@
       <c r="H14" t="n">
         <v>7.9</v>
       </c>
-      <c r="I14" t="n">
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J14" t="n">
         <v>15558528</v>
       </c>
-      <c r="J14" t="n">
+      <c r="K14" t="n">
         <v>5763524</v>
       </c>
-      <c r="K14" t="n">
+      <c r="L14" t="n">
         <v>989923</v>
       </c>
-      <c r="L14" t="n">
+      <c r="M14" t="n">
         <v>6248596</v>
       </c>
-      <c r="M14" t="n">
+      <c r="N14" t="n">
         <v>13316265</v>
       </c>
-      <c r="N14" t="n">
+      <c r="O14" t="n">
         <v>12254653</v>
       </c>
     </row>
@@ -1106,22 +1176,27 @@
       <c r="H15" t="n">
         <v>7.9</v>
       </c>
-      <c r="I15" t="n">
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J15" t="n">
         <v>15558528</v>
       </c>
-      <c r="J15" t="n">
+      <c r="K15" t="n">
         <v>5654090</v>
       </c>
-      <c r="K15" t="n">
+      <c r="L15" t="n">
         <v>975365</v>
       </c>
-      <c r="L15" t="n">
+      <c r="M15" t="n">
         <v>5994588</v>
       </c>
-      <c r="M15" t="n">
+      <c r="N15" t="n">
         <v>13168306</v>
       </c>
-      <c r="N15" t="n">
+      <c r="O15" t="n">
         <v>12254653</v>
       </c>
     </row>
@@ -1150,22 +1225,27 @@
       <c r="H16" t="n">
         <v>7.8</v>
       </c>
-      <c r="I16" t="n">
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J16" t="n">
         <v>15366448</v>
       </c>
-      <c r="J16" t="n">
+      <c r="K16" t="n">
         <v>5763524</v>
       </c>
-      <c r="K16" t="n">
+      <c r="L16" t="n">
         <v>1062712</v>
       </c>
-      <c r="L16" t="n">
+      <c r="M16" t="n">
         <v>5892985</v>
       </c>
-      <c r="M16" t="n">
+      <c r="N16" t="n">
         <v>13020348</v>
       </c>
-      <c r="N16" t="n">
+      <c r="O16" t="n">
         <v>12099531</v>
       </c>
     </row>
@@ -1194,22 +1274,27 @@
       <c r="H17" t="n">
         <v>8</v>
       </c>
-      <c r="I17" t="n">
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J17" t="n">
         <v>15558528</v>
       </c>
-      <c r="J17" t="n">
+      <c r="K17" t="n">
         <v>6018870</v>
       </c>
-      <c r="K17" t="n">
+      <c r="L17" t="n">
         <v>946250</v>
       </c>
-      <c r="L17" t="n">
+      <c r="M17" t="n">
         <v>6045390</v>
       </c>
-      <c r="M17" t="n">
+      <c r="N17" t="n">
         <v>13168306</v>
       </c>
-      <c r="N17" t="n">
+      <c r="O17" t="n">
         <v>12409776</v>
       </c>
     </row>
@@ -1238,22 +1323,27 @@
       <c r="H18" t="n">
         <v>8</v>
       </c>
-      <c r="I18" t="n">
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J18" t="n">
         <v>15174367</v>
       </c>
-      <c r="J18" t="n">
+      <c r="K18" t="n">
         <v>5945914</v>
       </c>
-      <c r="K18" t="n">
+      <c r="L18" t="n">
         <v>1048154</v>
       </c>
-      <c r="L18" t="n">
+      <c r="M18" t="n">
         <v>5892985</v>
       </c>
-      <c r="M18" t="n">
+      <c r="N18" t="n">
         <v>13020348</v>
       </c>
-      <c r="N18" t="n">
+      <c r="O18" t="n">
         <v>12409776</v>
       </c>
     </row>
@@ -1282,22 +1372,27 @@
       <c r="H19" t="n">
         <v>8</v>
       </c>
-      <c r="I19" t="n">
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J19" t="n">
         <v>15558528</v>
       </c>
-      <c r="J19" t="n">
+      <c r="K19" t="n">
         <v>5909436</v>
       </c>
-      <c r="K19" t="n">
+      <c r="L19" t="n">
         <v>946250</v>
       </c>
-      <c r="L19" t="n">
+      <c r="M19" t="n">
         <v>5842184</v>
       </c>
-      <c r="M19" t="n">
+      <c r="N19" t="n">
         <v>13316265</v>
       </c>
-      <c r="N19" t="n">
+      <c r="O19" t="n">
         <v>12409776</v>
       </c>
     </row>
@@ -1326,22 +1421,27 @@
       <c r="H20" t="n">
         <v>7.9</v>
       </c>
-      <c r="I20" t="n">
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J20" t="n">
         <v>15366448</v>
       </c>
-      <c r="J20" t="n">
+      <c r="K20" t="n">
         <v>5800002</v>
       </c>
-      <c r="K20" t="n">
+      <c r="L20" t="n">
         <v>1077269</v>
       </c>
-      <c r="L20" t="n">
+      <c r="M20" t="n">
         <v>5689779</v>
       </c>
-      <c r="M20" t="n">
+      <c r="N20" t="n">
         <v>13020348</v>
       </c>
-      <c r="N20" t="n">
+      <c r="O20" t="n">
         <v>12254653</v>
       </c>
     </row>
@@ -1370,22 +1470,27 @@
       <c r="H21" t="n">
         <v>7.9</v>
       </c>
-      <c r="I21" t="n">
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J21" t="n">
         <v>15174367</v>
       </c>
-      <c r="J21" t="n">
+      <c r="K21" t="n">
         <v>5982391</v>
       </c>
-      <c r="K21" t="n">
+      <c r="L21" t="n">
         <v>1048154</v>
       </c>
-      <c r="L21" t="n">
+      <c r="M21" t="n">
         <v>5689779</v>
       </c>
-      <c r="M21" t="n">
+      <c r="N21" t="n">
         <v>12872389</v>
       </c>
-      <c r="N21" t="n">
+      <c r="O21" t="n">
         <v>12254653</v>
       </c>
     </row>
@@ -1414,22 +1519,27 @@
       <c r="H22" t="n">
         <v>8.199999999999999</v>
       </c>
-      <c r="I22" t="n">
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J22" t="n">
         <v>15174367</v>
       </c>
-      <c r="J22" t="n">
+      <c r="K22" t="n">
         <v>5800002</v>
       </c>
-      <c r="K22" t="n">
+      <c r="L22" t="n">
         <v>1164616</v>
       </c>
-      <c r="L22" t="n">
+      <c r="M22" t="n">
         <v>5689779</v>
       </c>
-      <c r="M22" t="n">
+      <c r="N22" t="n">
         <v>12872389</v>
       </c>
-      <c r="N22" t="n">
+      <c r="O22" t="n">
         <v>12720020</v>
       </c>
     </row>
@@ -1458,22 +1568,27 @@
       <c r="H23" t="n">
         <v>7.8</v>
       </c>
-      <c r="I23" t="n">
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J23" t="n">
         <v>15174367</v>
       </c>
-      <c r="J23" t="n">
+      <c r="K23" t="n">
         <v>5325788</v>
       </c>
-      <c r="K23" t="n">
+      <c r="L23" t="n">
         <v>1077269</v>
       </c>
-      <c r="L23" t="n">
+      <c r="M23" t="n">
         <v>5740580</v>
       </c>
-      <c r="M23" t="n">
+      <c r="N23" t="n">
         <v>12724430</v>
       </c>
-      <c r="N23" t="n">
+      <c r="O23" t="n">
         <v>12099531</v>
       </c>
     </row>
@@ -1502,22 +1617,27 @@
       <c r="H24" t="n">
         <v>7.8</v>
       </c>
-      <c r="I24" t="n">
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J24" t="n">
         <v>14790206</v>
       </c>
-      <c r="J24" t="n">
+      <c r="K24" t="n">
         <v>5690568</v>
       </c>
-      <c r="K24" t="n">
+      <c r="L24" t="n">
         <v>931692</v>
       </c>
-      <c r="L24" t="n">
+      <c r="M24" t="n">
         <v>5689779</v>
       </c>
-      <c r="M24" t="n">
+      <c r="N24" t="n">
         <v>12132596</v>
       </c>
-      <c r="N24" t="n">
+      <c r="O24" t="n">
         <v>12099531</v>
       </c>
     </row>
@@ -1546,22 +1666,27 @@
       <c r="H25" t="n">
         <v>7.8</v>
       </c>
-      <c r="I25" t="n">
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J25" t="n">
         <v>14406045</v>
       </c>
-      <c r="J25" t="n">
+      <c r="K25" t="n">
         <v>5617612</v>
       </c>
-      <c r="K25" t="n">
+      <c r="L25" t="n">
         <v>989923</v>
       </c>
-      <c r="L25" t="n">
+      <c r="M25" t="n">
         <v>5638977</v>
       </c>
-      <c r="M25" t="n">
+      <c r="N25" t="n">
         <v>11836680</v>
       </c>
-      <c r="N25" t="n">
+      <c r="O25" t="n">
         <v>12099531</v>
       </c>
     </row>
@@ -1590,22 +1715,27 @@
       <c r="H26" t="n">
         <v>7.6</v>
       </c>
-      <c r="I26" t="n">
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J26" t="n">
         <v>14230570</v>
       </c>
-      <c r="J26" t="n">
+      <c r="K26" t="n">
         <v>5004460</v>
       </c>
-      <c r="K26" t="n">
+      <c r="L26" t="n">
         <v>1009549</v>
       </c>
-      <c r="L26" t="n">
+      <c r="M26" t="n">
         <v>5539753</v>
       </c>
-      <c r="M26" t="n">
+      <c r="N26" t="n">
         <v>11482609</v>
       </c>
-      <c r="N26" t="n">
+      <c r="O26" t="n">
         <v>11875136</v>
       </c>
     </row>
@@ -1634,22 +1764,27 @@
       <c r="H27" t="n">
         <v>7.6</v>
       </c>
-      <c r="I27" t="n">
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J27" t="n">
         <v>14230570</v>
       </c>
-      <c r="J27" t="n">
+      <c r="K27" t="n">
         <v>5151650</v>
       </c>
-      <c r="K27" t="n">
+      <c r="L27" t="n">
         <v>934209</v>
       </c>
-      <c r="L27" t="n">
+      <c r="M27" t="n">
         <v>5643300</v>
       </c>
-      <c r="M27" t="n">
+      <c r="N27" t="n">
         <v>11482609</v>
       </c>
-      <c r="N27" t="n">
+      <c r="O27" t="n">
         <v>11875136</v>
       </c>
     </row>
@@ -1678,22 +1813,27 @@
       <c r="H28" t="n">
         <v>7.400000000000001</v>
       </c>
-      <c r="I28" t="n">
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J28" t="n">
         <v>14038265</v>
       </c>
-      <c r="J28" t="n">
+      <c r="K28" t="n">
         <v>5151650</v>
       </c>
-      <c r="K28" t="n">
+      <c r="L28" t="n">
         <v>964345</v>
       </c>
-      <c r="L28" t="n">
+      <c r="M28" t="n">
         <v>5487980</v>
       </c>
-      <c r="M28" t="n">
+      <c r="N28" t="n">
         <v>11482609</v>
       </c>
-      <c r="N28" t="n">
+      <c r="O28" t="n">
         <v>11562633</v>
       </c>
     </row>
@@ -1722,22 +1862,27 @@
       <c r="H29" t="n">
         <v>7.400000000000001</v>
       </c>
-      <c r="I29" t="n">
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J29" t="n">
         <v>14230570</v>
       </c>
-      <c r="J29" t="n">
+      <c r="K29" t="n">
         <v>4894067</v>
       </c>
-      <c r="K29" t="n">
+      <c r="L29" t="n">
         <v>813666</v>
       </c>
-      <c r="L29" t="n">
+      <c r="M29" t="n">
         <v>5332660</v>
       </c>
-      <c r="M29" t="n">
+      <c r="N29" t="n">
         <v>11333484</v>
       </c>
-      <c r="N29" t="n">
+      <c r="O29" t="n">
         <v>11562633</v>
       </c>
     </row>
@@ -1766,22 +1911,27 @@
       <c r="H30" t="n">
         <v>7.400000000000001</v>
       </c>
-      <c r="I30" t="n">
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J30" t="n">
         <v>14230570</v>
       </c>
-      <c r="J30" t="n">
+      <c r="K30" t="n">
         <v>4967662</v>
       </c>
-      <c r="K30" t="n">
+      <c r="L30" t="n">
         <v>828734</v>
       </c>
-      <c r="L30" t="n">
+      <c r="M30" t="n">
         <v>5643300</v>
       </c>
-      <c r="M30" t="n">
+      <c r="N30" t="n">
         <v>11482609</v>
       </c>
-      <c r="N30" t="n">
+      <c r="O30" t="n">
         <v>11562633</v>
       </c>
     </row>
@@ -1810,22 +1960,27 @@
       <c r="H31" t="n">
         <v>7.400000000000001</v>
       </c>
-      <c r="I31" t="n">
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J31" t="n">
         <v>14038265</v>
       </c>
-      <c r="J31" t="n">
+      <c r="K31" t="n">
         <v>5335637</v>
       </c>
-      <c r="K31" t="n">
+      <c r="L31" t="n">
         <v>919141</v>
       </c>
-      <c r="L31" t="n">
+      <c r="M31" t="n">
         <v>5643300</v>
       </c>
-      <c r="M31" t="n">
+      <c r="N31" t="n">
         <v>11482609</v>
       </c>
-      <c r="N31" t="n">
+      <c r="O31" t="n">
         <v>11562633</v>
       </c>
     </row>
@@ -1854,22 +2009,27 @@
       <c r="H32" t="n">
         <v>7.400000000000001</v>
       </c>
-      <c r="I32" t="n">
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J32" t="n">
         <v>14038265</v>
       </c>
-      <c r="J32" t="n">
+      <c r="K32" t="n">
         <v>5225244</v>
       </c>
-      <c r="K32" t="n">
+      <c r="L32" t="n">
         <v>889006</v>
       </c>
-      <c r="L32" t="n">
+      <c r="M32" t="n">
         <v>5280886</v>
       </c>
-      <c r="M32" t="n">
+      <c r="N32" t="n">
         <v>11482609</v>
       </c>
-      <c r="N32" t="n">
+      <c r="O32" t="n">
         <v>11562633</v>
       </c>
     </row>
@@ -1898,22 +2058,27 @@
       <c r="H33" t="n">
         <v>7.3</v>
       </c>
-      <c r="I33" t="n">
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J33" t="n">
         <v>13845960</v>
       </c>
-      <c r="J33" t="n">
+      <c r="K33" t="n">
         <v>5078055</v>
       </c>
-      <c r="K33" t="n">
+      <c r="L33" t="n">
         <v>889006</v>
       </c>
-      <c r="L33" t="n">
+      <c r="M33" t="n">
         <v>5229113</v>
       </c>
-      <c r="M33" t="n">
+      <c r="N33" t="n">
         <v>11333484</v>
       </c>
-      <c r="N33" t="n">
+      <c r="O33" t="n">
         <v>11406381</v>
       </c>
     </row>
@@ -1942,22 +2107,27 @@
       <c r="H34" t="n">
         <v>7.1</v>
       </c>
-      <c r="I34" t="n">
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J34" t="n">
         <v>13461350</v>
       </c>
-      <c r="J34" t="n">
+      <c r="K34" t="n">
         <v>5004460</v>
       </c>
-      <c r="K34" t="n">
+      <c r="L34" t="n">
         <v>738327</v>
       </c>
-      <c r="L34" t="n">
+      <c r="M34" t="n">
         <v>5022019</v>
       </c>
-      <c r="M34" t="n">
+      <c r="N34" t="n">
         <v>10886110</v>
       </c>
-      <c r="N34" t="n">
+      <c r="O34" t="n">
         <v>11093877</v>
       </c>
     </row>
@@ -1986,22 +2156,27 @@
       <c r="H35" t="n">
         <v>7.1</v>
       </c>
-      <c r="I35" t="n">
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J35" t="n">
         <v>13269045</v>
       </c>
-      <c r="J35" t="n">
+      <c r="K35" t="n">
         <v>5188447</v>
       </c>
-      <c r="K35" t="n">
+      <c r="L35" t="n">
         <v>738327</v>
       </c>
-      <c r="L35" t="n">
+      <c r="M35" t="n">
         <v>5177340</v>
       </c>
-      <c r="M35" t="n">
+      <c r="N35" t="n">
         <v>10736985</v>
       </c>
-      <c r="N35" t="n">
+      <c r="O35" t="n">
         <v>11093877</v>
       </c>
     </row>
@@ -2030,22 +2205,27 @@
       <c r="H36" t="n">
         <v>7.000000000000001</v>
       </c>
-      <c r="I36" t="n">
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J36" t="n">
         <v>13076740</v>
       </c>
-      <c r="J36" t="n">
+      <c r="K36" t="n">
         <v>4894067</v>
       </c>
-      <c r="K36" t="n">
+      <c r="L36" t="n">
         <v>949277</v>
       </c>
-      <c r="L36" t="n">
+      <c r="M36" t="n">
         <v>5125566</v>
       </c>
-      <c r="M36" t="n">
+      <c r="N36" t="n">
         <v>10736985</v>
       </c>
-      <c r="N36" t="n">
+      <c r="O36" t="n">
         <v>10937626</v>
       </c>
     </row>
@@ -2074,22 +2254,27 @@
       <c r="H37" t="n">
         <v>7.400000000000001</v>
       </c>
-      <c r="I37" t="n">
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J37" t="n">
         <v>13269045</v>
       </c>
-      <c r="J37" t="n">
+      <c r="K37" t="n">
         <v>5151650</v>
       </c>
-      <c r="K37" t="n">
+      <c r="L37" t="n">
         <v>994481</v>
       </c>
-      <c r="L37" t="n">
+      <c r="M37" t="n">
         <v>4970246</v>
       </c>
-      <c r="M37" t="n">
+      <c r="N37" t="n">
         <v>10736985</v>
       </c>
-      <c r="N37" t="n">
+      <c r="O37" t="n">
         <v>11562633</v>
       </c>
     </row>
@@ -2118,22 +2303,27 @@
       <c r="H38" t="n">
         <v>7.200000000000001</v>
       </c>
-      <c r="I38" t="n">
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J38" t="n">
         <v>13658944</v>
       </c>
-      <c r="J38" t="n">
+      <c r="K38" t="n">
         <v>5085796</v>
       </c>
-      <c r="K38" t="n">
+      <c r="L38" t="n">
         <v>992364</v>
       </c>
-      <c r="L38" t="n">
+      <c r="M38" t="n">
         <v>5118195</v>
       </c>
-      <c r="M38" t="n">
+      <c r="N38" t="n">
         <v>11272372</v>
       </c>
-      <c r="N38" t="n">
+      <c r="O38" t="n">
         <v>11318918</v>
       </c>
     </row>
@@ -2162,22 +2352,27 @@
       <c r="H39" t="n">
         <v>7.000000000000001</v>
       </c>
-      <c r="I39" t="n">
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J39" t="n">
         <v>13081806</v>
       </c>
-      <c r="J39" t="n">
+      <c r="K39" t="n">
         <v>5122918</v>
       </c>
-      <c r="K39" t="n">
+      <c r="L39" t="n">
         <v>930342</v>
       </c>
-      <c r="L39" t="n">
+      <c r="M39" t="n">
         <v>5118195</v>
       </c>
-      <c r="M39" t="n">
+      <c r="N39" t="n">
         <v>10520881</v>
       </c>
-      <c r="N39" t="n">
+      <c r="O39" t="n">
         <v>11004504</v>
       </c>
     </row>
@@ -2206,22 +2401,27 @@
       <c r="H40" t="n">
         <v>6.9</v>
       </c>
-      <c r="I40" t="n">
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J40" t="n">
         <v>12889426</v>
       </c>
-      <c r="J40" t="n">
+      <c r="K40" t="n">
         <v>4825938</v>
       </c>
-      <c r="K40" t="n">
+      <c r="L40" t="n">
         <v>790790</v>
       </c>
-      <c r="L40" t="n">
+      <c r="M40" t="n">
         <v>4907135</v>
       </c>
-      <c r="M40" t="n">
+      <c r="N40" t="n">
         <v>10370582</v>
       </c>
-      <c r="N40" t="n">
+      <c r="O40" t="n">
         <v>10847296</v>
       </c>
     </row>
@@ -2250,22 +2450,27 @@
       <c r="H41" t="n">
         <v>6.7</v>
       </c>
-      <c r="I41" t="n">
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J41" t="n">
         <v>12889426</v>
       </c>
-      <c r="J41" t="n">
+      <c r="K41" t="n">
         <v>4937305</v>
       </c>
-      <c r="K41" t="n">
+      <c r="L41" t="n">
         <v>821802</v>
       </c>
-      <c r="L41" t="n">
+      <c r="M41" t="n">
         <v>4748841</v>
       </c>
-      <c r="M41" t="n">
+      <c r="N41" t="n">
         <v>10821477</v>
       </c>
-      <c r="N41" t="n">
+      <c r="O41" t="n">
         <v>10532882</v>
       </c>
     </row>
@@ -2294,22 +2499,27 @@
       <c r="H42" t="n">
         <v>6.5</v>
       </c>
-      <c r="I42" t="n">
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J42" t="n">
         <v>12889426</v>
       </c>
-      <c r="J42" t="n">
+      <c r="K42" t="n">
         <v>4974428</v>
       </c>
-      <c r="K42" t="n">
+      <c r="L42" t="n">
         <v>697756</v>
       </c>
-      <c r="L42" t="n">
+      <c r="M42" t="n">
         <v>4748841</v>
       </c>
-      <c r="M42" t="n">
+      <c r="N42" t="n">
         <v>10671179</v>
       </c>
-      <c r="N42" t="n">
+      <c r="O42" t="n">
         <v>10218468</v>
       </c>
     </row>
@@ -2338,22 +2548,27 @@
       <c r="H43" t="n">
         <v>6.800000000000001</v>
       </c>
-      <c r="I43" t="n">
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J43" t="n">
         <v>12697047</v>
       </c>
-      <c r="J43" t="n">
+      <c r="K43" t="n">
         <v>5271409</v>
       </c>
-      <c r="K43" t="n">
+      <c r="L43" t="n">
         <v>728767</v>
       </c>
-      <c r="L43" t="n">
+      <c r="M43" t="n">
         <v>4801605</v>
       </c>
-      <c r="M43" t="n">
+      <c r="N43" t="n">
         <v>10520881</v>
       </c>
-      <c r="N43" t="n">
+      <c r="O43" t="n">
         <v>10690089</v>
       </c>
     </row>
@@ -2382,22 +2597,27 @@
       <c r="H44" t="n">
         <v>6.3</v>
       </c>
-      <c r="I44" t="n">
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J44" t="n">
         <v>12504667</v>
       </c>
-      <c r="J44" t="n">
+      <c r="K44" t="n">
         <v>4677447</v>
       </c>
-      <c r="K44" t="n">
+      <c r="L44" t="n">
         <v>821802</v>
       </c>
-      <c r="L44" t="n">
+      <c r="M44" t="n">
         <v>4959900</v>
       </c>
-      <c r="M44" t="n">
+      <c r="N44" t="n">
         <v>10520881</v>
       </c>
-      <c r="N44" t="n">
+      <c r="O44" t="n">
         <v>9904053</v>
       </c>
     </row>
@@ -2426,22 +2646,27 @@
       <c r="H45" t="n">
         <v>6.2</v>
       </c>
-      <c r="I45" t="n">
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J45" t="n">
         <v>12312288</v>
       </c>
-      <c r="J45" t="n">
+      <c r="K45" t="n">
         <v>4751692</v>
       </c>
-      <c r="K45" t="n">
+      <c r="L45" t="n">
         <v>790790</v>
       </c>
-      <c r="L45" t="n">
+      <c r="M45" t="n">
         <v>4854370</v>
       </c>
-      <c r="M45" t="n">
+      <c r="N45" t="n">
         <v>10671179</v>
       </c>
-      <c r="N45" t="n">
+      <c r="O45" t="n">
         <v>9746846</v>
       </c>
     </row>
@@ -2470,22 +2695,27 @@
       <c r="H46" t="n">
         <v>6.2</v>
       </c>
-      <c r="I46" t="n">
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J46" t="n">
         <v>12119908</v>
       </c>
-      <c r="J46" t="n">
+      <c r="K46" t="n">
         <v>4825938</v>
       </c>
-      <c r="K46" t="n">
+      <c r="L46" t="n">
         <v>837307</v>
       </c>
-      <c r="L46" t="n">
+      <c r="M46" t="n">
         <v>4643311</v>
       </c>
-      <c r="M46" t="n">
+      <c r="N46" t="n">
         <v>10671179</v>
       </c>
-      <c r="N46" t="n">
+      <c r="O46" t="n">
         <v>9746846</v>
       </c>
     </row>
@@ -2514,22 +2744,27 @@
       <c r="H47" t="n">
         <v>6.3</v>
       </c>
-      <c r="I47" t="n">
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J47" t="n">
         <v>12119908</v>
       </c>
-      <c r="J47" t="n">
+      <c r="K47" t="n">
         <v>4751692</v>
       </c>
-      <c r="K47" t="n">
+      <c r="L47" t="n">
         <v>837307</v>
       </c>
-      <c r="L47" t="n">
+      <c r="M47" t="n">
         <v>4801605</v>
       </c>
-      <c r="M47" t="n">
+      <c r="N47" t="n">
         <v>10370582</v>
       </c>
-      <c r="N47" t="n">
+      <c r="O47" t="n">
         <v>9904053</v>
       </c>
     </row>
@@ -2558,22 +2793,27 @@
       <c r="H48" t="n">
         <v>6.2</v>
       </c>
-      <c r="I48" t="n">
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J48" t="n">
         <v>11735149</v>
       </c>
-      <c r="J48" t="n">
+      <c r="K48" t="n">
         <v>4566079</v>
       </c>
-      <c r="K48" t="n">
+      <c r="L48" t="n">
         <v>806296</v>
       </c>
-      <c r="L48" t="n">
+      <c r="M48" t="n">
         <v>4590546</v>
       </c>
-      <c r="M48" t="n">
+      <c r="N48" t="n">
         <v>9919687</v>
       </c>
-      <c r="N48" t="n">
+      <c r="O48" t="n">
         <v>9746846</v>
       </c>
     </row>
@@ -2602,22 +2842,27 @@
       <c r="H49" t="n">
         <v>6.1</v>
       </c>
-      <c r="I49" t="n">
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J49" t="n">
         <v>11350390</v>
       </c>
-      <c r="J49" t="n">
+      <c r="K49" t="n">
         <v>4417589</v>
       </c>
-      <c r="K49" t="n">
+      <c r="L49" t="n">
         <v>666745</v>
       </c>
-      <c r="L49" t="n">
+      <c r="M49" t="n">
         <v>4379486</v>
       </c>
-      <c r="M49" t="n">
+      <c r="N49" t="n">
         <v>9468792</v>
       </c>
-      <c r="N49" t="n">
+      <c r="O49" t="n">
         <v>9589639</v>
       </c>
     </row>
@@ -2646,22 +2891,27 @@
       <c r="H50" t="n">
         <v>5.8</v>
       </c>
-      <c r="I50" t="n">
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J50" t="n">
         <v>10967917</v>
       </c>
-      <c r="J50" t="n">
+      <c r="K50" t="n">
         <v>4549527</v>
       </c>
-      <c r="K50" t="n">
+      <c r="L50" t="n">
         <v>759355</v>
       </c>
-      <c r="L50" t="n">
+      <c r="M50" t="n">
         <v>4486946</v>
       </c>
-      <c r="M50" t="n">
+      <c r="N50" t="n">
         <v>9395405</v>
       </c>
-      <c r="N50" t="n">
+      <c r="O50" t="n">
         <v>9203057</v>
       </c>
     </row>
@@ -2690,22 +2940,27 @@
       <c r="H51" t="n">
         <v>5.9</v>
       </c>
-      <c r="I51" t="n">
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J51" t="n">
         <v>11160336</v>
       </c>
-      <c r="J51" t="n">
+      <c r="K51" t="n">
         <v>4436729</v>
       </c>
-      <c r="K51" t="n">
+      <c r="L51" t="n">
         <v>953233</v>
       </c>
-      <c r="L51" t="n">
+      <c r="M51" t="n">
         <v>4432887</v>
       </c>
-      <c r="M51" t="n">
+      <c r="N51" t="n">
         <v>9546944</v>
       </c>
-      <c r="N51" t="n">
+      <c r="O51" t="n">
         <v>9361730</v>
       </c>
     </row>
@@ -2734,22 +2989,27 @@
       <c r="H52" t="n">
         <v>6.2</v>
       </c>
-      <c r="I52" t="n">
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J52" t="n">
         <v>11160336</v>
       </c>
-      <c r="J52" t="n">
+      <c r="K52" t="n">
         <v>4549527</v>
       </c>
-      <c r="K52" t="n">
+      <c r="L52" t="n">
         <v>888607</v>
       </c>
-      <c r="L52" t="n">
+      <c r="M52" t="n">
         <v>4270708</v>
       </c>
-      <c r="M52" t="n">
+      <c r="N52" t="n">
         <v>9243866</v>
       </c>
-      <c r="N52" t="n">
+      <c r="O52" t="n">
         <v>9837750</v>
       </c>
     </row>
@@ -2778,22 +3038,27 @@
       <c r="H53" t="n">
         <v>5.6</v>
       </c>
-      <c r="I53" t="n">
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J53" t="n">
         <v>10198238</v>
       </c>
-      <c r="J53" t="n">
+      <c r="K53" t="n">
         <v>4361530</v>
       </c>
-      <c r="K53" t="n">
+      <c r="L53" t="n">
         <v>953233</v>
       </c>
-      <c r="L53" t="n">
+      <c r="M53" t="n">
         <v>3892291</v>
       </c>
-      <c r="M53" t="n">
+      <c r="N53" t="n">
         <v>8940789</v>
       </c>
-      <c r="N53" t="n">
+      <c r="O53" t="n">
         <v>8885710</v>
       </c>
     </row>
@@ -2822,22 +3087,27 @@
       <c r="H54" t="n">
         <v>5.8</v>
       </c>
-      <c r="I54" t="n">
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J54" t="n">
         <v>10390658</v>
       </c>
-      <c r="J54" t="n">
+      <c r="K54" t="n">
         <v>4286331</v>
       </c>
-      <c r="K54" t="n">
+      <c r="L54" t="n">
         <v>920920</v>
       </c>
-      <c r="L54" t="n">
+      <c r="M54" t="n">
         <v>4162589</v>
       </c>
-      <c r="M54" t="n">
+      <c r="N54" t="n">
         <v>8940789</v>
       </c>
-      <c r="N54" t="n">
+      <c r="O54" t="n">
         <v>9203057</v>
       </c>
     </row>
@@ -2866,22 +3136,27 @@
       <c r="H55" t="n">
         <v>5.3</v>
       </c>
-      <c r="I55" t="n">
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J55" t="n">
         <v>10198238</v>
       </c>
-      <c r="J55" t="n">
+      <c r="K55" t="n">
         <v>4135934</v>
       </c>
-      <c r="K55" t="n">
+      <c r="L55" t="n">
         <v>759355</v>
       </c>
-      <c r="L55" t="n">
+      <c r="M55" t="n">
         <v>4216648</v>
       </c>
-      <c r="M55" t="n">
+      <c r="N55" t="n">
         <v>8637711</v>
       </c>
-      <c r="N55" t="n">
+      <c r="O55" t="n">
         <v>8409690</v>
       </c>
     </row>
@@ -2910,22 +3185,27 @@
       <c r="H56" t="n">
         <v>5.6</v>
       </c>
-      <c r="I56" t="n">
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J56" t="n">
         <v>10198238</v>
       </c>
-      <c r="J56" t="n">
+      <c r="K56" t="n">
         <v>4361530</v>
       </c>
-      <c r="K56" t="n">
+      <c r="L56" t="n">
         <v>678573</v>
       </c>
-      <c r="L56" t="n">
+      <c r="M56" t="n">
         <v>4162589</v>
       </c>
-      <c r="M56" t="n">
+      <c r="N56" t="n">
         <v>8637711</v>
       </c>
-      <c r="N56" t="n">
+      <c r="O56" t="n">
         <v>8885710</v>
       </c>
     </row>
@@ -2954,22 +3234,27 @@
       <c r="H57" t="n">
         <v>5.6</v>
       </c>
-      <c r="I57" t="n">
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J57" t="n">
         <v>10198238</v>
       </c>
-      <c r="J57" t="n">
+      <c r="K57" t="n">
         <v>4286331</v>
       </c>
-      <c r="K57" t="n">
+      <c r="L57" t="n">
         <v>727042</v>
       </c>
-      <c r="L57" t="n">
+      <c r="M57" t="n">
         <v>4000410</v>
       </c>
-      <c r="M57" t="n">
+      <c r="N57" t="n">
         <v>8637711</v>
       </c>
-      <c r="N57" t="n">
+      <c r="O57" t="n">
         <v>8885710</v>
       </c>
     </row>
@@ -2998,22 +3283,27 @@
       <c r="H58" t="n">
         <v>5.5</v>
       </c>
-      <c r="I58" t="n">
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J58" t="n">
         <v>9813399</v>
       </c>
-      <c r="J58" t="n">
+      <c r="K58" t="n">
         <v>4135934</v>
       </c>
-      <c r="K58" t="n">
+      <c r="L58" t="n">
         <v>710886</v>
       </c>
-      <c r="L58" t="n">
+      <c r="M58" t="n">
         <v>3676052</v>
       </c>
-      <c r="M58" t="n">
+      <c r="N58" t="n">
         <v>8031556</v>
       </c>
-      <c r="N58" t="n">
+      <c r="O58" t="n">
         <v>8727037</v>
       </c>
     </row>
@@ -3042,22 +3332,27 @@
       <c r="H59" t="n">
         <v>5.4</v>
       </c>
-      <c r="I59" t="n">
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J59" t="n">
         <v>9428560</v>
       </c>
-      <c r="J59" t="n">
+      <c r="K59" t="n">
         <v>3985536</v>
       </c>
-      <c r="K59" t="n">
+      <c r="L59" t="n">
         <v>823981</v>
       </c>
-      <c r="L59" t="n">
+      <c r="M59" t="n">
         <v>3676052</v>
       </c>
-      <c r="M59" t="n">
+      <c r="N59" t="n">
         <v>7728478</v>
       </c>
-      <c r="N59" t="n">
+      <c r="O59" t="n">
         <v>8568363</v>
       </c>
     </row>
@@ -3086,22 +3381,27 @@
       <c r="H60" t="n">
         <v>5.3</v>
       </c>
-      <c r="I60" t="n">
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J60" t="n">
         <v>9620980</v>
       </c>
-      <c r="J60" t="n">
+      <c r="K60" t="n">
         <v>4098334</v>
       </c>
-      <c r="K60" t="n">
+      <c r="L60" t="n">
         <v>775512</v>
       </c>
-      <c r="L60" t="n">
+      <c r="M60" t="n">
         <v>3567933</v>
       </c>
-      <c r="M60" t="n">
+      <c r="N60" t="n">
         <v>8183095</v>
       </c>
-      <c r="N60" t="n">
+      <c r="O60" t="n">
         <v>8409690</v>
       </c>
     </row>
@@ -3130,22 +3430,27 @@
       <c r="H61" t="n">
         <v>5.1</v>
       </c>
-      <c r="I61" t="n">
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J61" t="n">
         <v>9043721</v>
       </c>
-      <c r="J61" t="n">
+      <c r="K61" t="n">
         <v>3985536</v>
       </c>
-      <c r="K61" t="n">
+      <c r="L61" t="n">
         <v>710886</v>
       </c>
-      <c r="L61" t="n">
+      <c r="M61" t="n">
         <v>3459814</v>
       </c>
-      <c r="M61" t="n">
+      <c r="N61" t="n">
         <v>7880017</v>
       </c>
-      <c r="N61" t="n">
+      <c r="O61" t="n">
         <v>8092343</v>
       </c>
     </row>
@@ -3174,22 +3479,27 @@
       <c r="H62" t="n">
         <v>5</v>
       </c>
-      <c r="I62" t="n">
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J62" t="n">
         <v>9437086</v>
       </c>
-      <c r="J62" t="n">
+      <c r="K62" t="n">
         <v>3906151</v>
       </c>
-      <c r="K62" t="n">
+      <c r="L62" t="n">
         <v>670212</v>
       </c>
-      <c r="L62" t="n">
+      <c r="M62" t="n">
         <v>3701167</v>
       </c>
-      <c r="M62" t="n">
+      <c r="N62" t="n">
         <v>8098389</v>
       </c>
-      <c r="N62" t="n">
+      <c r="O62" t="n">
         <v>7998910</v>
       </c>
     </row>
@@ -3218,22 +3528,27 @@
       <c r="H63" t="n">
         <v>4.9</v>
       </c>
-      <c r="I63" t="n">
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J63" t="n">
         <v>9051899</v>
       </c>
-      <c r="J63" t="n">
+      <c r="K63" t="n">
         <v>3830303</v>
       </c>
-      <c r="K63" t="n">
+      <c r="L63" t="n">
         <v>670212</v>
       </c>
-      <c r="L63" t="n">
+      <c r="M63" t="n">
         <v>3756408</v>
       </c>
-      <c r="M63" t="n">
+      <c r="N63" t="n">
         <v>7945589</v>
       </c>
-      <c r="N63" t="n">
+      <c r="O63" t="n">
         <v>7838931</v>
       </c>
     </row>
@@ -3262,22 +3577,27 @@
       <c r="H64" t="n">
         <v>4.9</v>
       </c>
-      <c r="I64" t="n">
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J64" t="n">
         <v>9244492</v>
       </c>
-      <c r="J64" t="n">
+      <c r="K64" t="n">
         <v>3754456</v>
       </c>
-      <c r="K64" t="n">
+      <c r="L64" t="n">
         <v>536169</v>
       </c>
-      <c r="L64" t="n">
+      <c r="M64" t="n">
         <v>3756408</v>
       </c>
-      <c r="M64" t="n">
+      <c r="N64" t="n">
         <v>7792789</v>
       </c>
-      <c r="N64" t="n">
+      <c r="O64" t="n">
         <v>7838931</v>
       </c>
     </row>
@@ -3306,22 +3626,27 @@
       <c r="H65" t="n">
         <v>5</v>
       </c>
-      <c r="I65" t="n">
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J65" t="n">
         <v>9051899</v>
       </c>
-      <c r="J65" t="n">
+      <c r="K65" t="n">
         <v>3678608</v>
       </c>
-      <c r="K65" t="n">
+      <c r="L65" t="n">
         <v>737233</v>
       </c>
-      <c r="L65" t="n">
+      <c r="M65" t="n">
         <v>3756408</v>
       </c>
-      <c r="M65" t="n">
+      <c r="N65" t="n">
         <v>7639990</v>
       </c>
-      <c r="N65" t="n">
+      <c r="O65" t="n">
         <v>7998910</v>
       </c>
     </row>
@@ -3350,22 +3675,27 @@
       <c r="H66" t="n">
         <v>5.1</v>
       </c>
-      <c r="I66" t="n">
+      <c r="I66" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J66" t="n">
         <v>9244492</v>
       </c>
-      <c r="J66" t="n">
+      <c r="K66" t="n">
         <v>3906151</v>
       </c>
-      <c r="K66" t="n">
+      <c r="L66" t="n">
         <v>686967</v>
       </c>
-      <c r="L66" t="n">
+      <c r="M66" t="n">
         <v>3756408</v>
       </c>
-      <c r="M66" t="n">
+      <c r="N66" t="n">
         <v>7945589</v>
       </c>
-      <c r="N66" t="n">
+      <c r="O66" t="n">
         <v>8158888</v>
       </c>
     </row>
@@ -3394,22 +3724,27 @@
       <c r="H67" t="n">
         <v>4.7</v>
       </c>
-      <c r="I67" t="n">
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J67" t="n">
         <v>8859305</v>
       </c>
-      <c r="J67" t="n">
+      <c r="K67" t="n">
         <v>3678608</v>
       </c>
-      <c r="K67" t="n">
+      <c r="L67" t="n">
         <v>653456</v>
       </c>
-      <c r="L67" t="n">
+      <c r="M67" t="n">
         <v>3701167</v>
       </c>
-      <c r="M67" t="n">
+      <c r="N67" t="n">
         <v>7334390</v>
       </c>
-      <c r="N67" t="n">
+      <c r="O67" t="n">
         <v>7518975</v>
       </c>
     </row>
@@ -3438,22 +3773,27 @@
       <c r="H68" t="n">
         <v>4.8</v>
       </c>
-      <c r="I68" t="n">
+      <c r="I68" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J68" t="n">
         <v>8666712</v>
       </c>
-      <c r="J68" t="n">
+      <c r="K68" t="n">
         <v>3451065</v>
       </c>
-      <c r="K68" t="n">
+      <c r="L68" t="n">
         <v>653456</v>
       </c>
-      <c r="L68" t="n">
+      <c r="M68" t="n">
         <v>3811649</v>
       </c>
-      <c r="M68" t="n">
+      <c r="N68" t="n">
         <v>7334390</v>
       </c>
-      <c r="N68" t="n">
+      <c r="O68" t="n">
         <v>7678953</v>
       </c>
     </row>
@@ -3482,22 +3822,27 @@
       <c r="H69" t="n">
         <v>4.6</v>
       </c>
-      <c r="I69" t="n">
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J69" t="n">
         <v>8474118</v>
       </c>
-      <c r="J69" t="n">
+      <c r="K69" t="n">
         <v>3564837</v>
       </c>
-      <c r="K69" t="n">
+      <c r="L69" t="n">
         <v>569680</v>
       </c>
-      <c r="L69" t="n">
+      <c r="M69" t="n">
         <v>3645925</v>
       </c>
-      <c r="M69" t="n">
+      <c r="N69" t="n">
         <v>7181590</v>
       </c>
-      <c r="N69" t="n">
+      <c r="O69" t="n">
         <v>7358997</v>
       </c>
     </row>
@@ -3526,22 +3871,27 @@
       <c r="H70" t="n">
         <v>4.6</v>
       </c>
-      <c r="I70" t="n">
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J70" t="n">
         <v>8474118</v>
       </c>
-      <c r="J70" t="n">
+      <c r="K70" t="n">
         <v>3526913</v>
       </c>
-      <c r="K70" t="n">
+      <c r="L70" t="n">
         <v>586435</v>
       </c>
-      <c r="L70" t="n">
+      <c r="M70" t="n">
         <v>3424960</v>
       </c>
-      <c r="M70" t="n">
+      <c r="N70" t="n">
         <v>7181590</v>
       </c>
-      <c r="N70" t="n">
+      <c r="O70" t="n">
         <v>7358997</v>
       </c>
     </row>
@@ -3570,22 +3920,27 @@
       <c r="H71" t="n">
         <v>4.6</v>
       </c>
-      <c r="I71" t="n">
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J71" t="n">
         <v>8474118</v>
       </c>
-      <c r="J71" t="n">
+      <c r="K71" t="n">
         <v>3413142</v>
       </c>
-      <c r="K71" t="n">
+      <c r="L71" t="n">
         <v>586435</v>
       </c>
-      <c r="L71" t="n">
+      <c r="M71" t="n">
         <v>3480201</v>
       </c>
-      <c r="M71" t="n">
+      <c r="N71" t="n">
         <v>7181590</v>
       </c>
-      <c r="N71" t="n">
+      <c r="O71" t="n">
         <v>7358997</v>
       </c>
     </row>
@@ -3614,22 +3969,27 @@
       <c r="H72" t="n">
         <v>4.6</v>
       </c>
-      <c r="I72" t="n">
+      <c r="I72" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J72" t="n">
         <v>8474118</v>
       </c>
-      <c r="J72" t="n">
+      <c r="K72" t="n">
         <v>3564837</v>
       </c>
-      <c r="K72" t="n">
+      <c r="L72" t="n">
         <v>653456</v>
       </c>
-      <c r="L72" t="n">
+      <c r="M72" t="n">
         <v>3535443</v>
       </c>
-      <c r="M72" t="n">
+      <c r="N72" t="n">
         <v>7334390</v>
       </c>
-      <c r="N72" t="n">
+      <c r="O72" t="n">
         <v>7358997</v>
       </c>
     </row>
@@ -3658,22 +4018,27 @@
       <c r="H73" t="n">
         <v>4.5</v>
       </c>
-      <c r="I73" t="n">
+      <c r="I73" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J73" t="n">
         <v>8474118</v>
       </c>
-      <c r="J73" t="n">
+      <c r="K73" t="n">
         <v>3223523</v>
       </c>
-      <c r="K73" t="n">
+      <c r="L73" t="n">
         <v>686967</v>
       </c>
-      <c r="L73" t="n">
+      <c r="M73" t="n">
         <v>3424960</v>
       </c>
-      <c r="M73" t="n">
+      <c r="N73" t="n">
         <v>7028790</v>
       </c>
-      <c r="N73" t="n">
+      <c r="O73" t="n">
         <v>7199019</v>
       </c>
     </row>
@@ -3702,22 +4067,27 @@
       <c r="H74" t="n">
         <v>4.5</v>
       </c>
-      <c r="I74" t="n">
+      <c r="I74" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J74" t="n">
         <v>8086575</v>
       </c>
-      <c r="J74" t="n">
+      <c r="K74" t="n">
         <v>3313107</v>
       </c>
-      <c r="K74" t="n">
+      <c r="L74" t="n">
         <v>612162</v>
       </c>
-      <c r="L74" t="n">
+      <c r="M74" t="n">
         <v>3256375</v>
       </c>
-      <c r="M74" t="n">
+      <c r="N74" t="n">
         <v>6764441</v>
       </c>
-      <c r="N74" t="n">
+      <c r="O74" t="n">
         <v>7232809</v>
       </c>
     </row>
@@ -3746,22 +4116,27 @@
       <c r="H75" t="n">
         <v>4.5</v>
       </c>
-      <c r="I75" t="n">
+      <c r="I75" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J75" t="n">
         <v>8279112</v>
       </c>
-      <c r="J75" t="n">
+      <c r="K75" t="n">
         <v>3236944</v>
       </c>
-      <c r="K75" t="n">
+      <c r="L75" t="n">
         <v>646171</v>
       </c>
-      <c r="L75" t="n">
+      <c r="M75" t="n">
         <v>3031797</v>
       </c>
-      <c r="M75" t="n">
+      <c r="N75" t="n">
         <v>6918178</v>
       </c>
-      <c r="N75" t="n">
+      <c r="O75" t="n">
         <v>7232809</v>
       </c>
     </row>
@@ -3790,22 +4165,27 @@
       <c r="H76" t="n">
         <v>4.6</v>
       </c>
-      <c r="I76" t="n">
+      <c r="I76" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J76" t="n">
         <v>8279112</v>
       </c>
-      <c r="J76" t="n">
+      <c r="K76" t="n">
         <v>3389271</v>
       </c>
-      <c r="K76" t="n">
+      <c r="L76" t="n">
         <v>663175</v>
       </c>
-      <c r="L76" t="n">
+      <c r="M76" t="n">
         <v>3087942</v>
       </c>
-      <c r="M76" t="n">
+      <c r="N76" t="n">
         <v>6918178</v>
       </c>
-      <c r="N76" t="n">
+      <c r="O76" t="n">
         <v>7393538</v>
       </c>
     </row>
@@ -3834,22 +4214,27 @@
       <c r="H77" t="n">
         <v>4.6</v>
       </c>
-      <c r="I77" t="n">
+      <c r="I77" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J77" t="n">
         <v>8471650</v>
       </c>
-      <c r="J77" t="n">
+      <c r="K77" t="n">
         <v>3351189</v>
       </c>
-      <c r="K77" t="n">
+      <c r="L77" t="n">
         <v>646171</v>
       </c>
-      <c r="L77" t="n">
+      <c r="M77" t="n">
         <v>3424808</v>
       </c>
-      <c r="M77" t="n">
+      <c r="N77" t="n">
         <v>7071915</v>
       </c>
-      <c r="N77" t="n">
+      <c r="O77" t="n">
         <v>7393538</v>
       </c>
     </row>
@@ -3878,22 +4263,27 @@
       <c r="H78" t="n">
         <v>4.3</v>
       </c>
-      <c r="I78" t="n">
+      <c r="I78" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J78" t="n">
         <v>8086575</v>
       </c>
-      <c r="J78" t="n">
+      <c r="K78" t="n">
         <v>3122699</v>
       </c>
-      <c r="K78" t="n">
+      <c r="L78" t="n">
         <v>714189</v>
       </c>
-      <c r="L78" t="n">
+      <c r="M78" t="n">
         <v>3144086</v>
       </c>
-      <c r="M78" t="n">
+      <c r="N78" t="n">
         <v>6918178</v>
       </c>
-      <c r="N78" t="n">
+      <c r="O78" t="n">
         <v>6911351</v>
       </c>
     </row>
@@ -3922,22 +4312,27 @@
       <c r="H79" t="n">
         <v>4.4</v>
       </c>
-      <c r="I79" t="n">
+      <c r="I79" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J79" t="n">
         <v>8279112</v>
       </c>
-      <c r="J79" t="n">
+      <c r="K79" t="n">
         <v>3351189</v>
       </c>
-      <c r="K79" t="n">
+      <c r="L79" t="n">
         <v>595157</v>
       </c>
-      <c r="L79" t="n">
+      <c r="M79" t="n">
         <v>3312519</v>
       </c>
-      <c r="M79" t="n">
+      <c r="N79" t="n">
         <v>6918178</v>
       </c>
-      <c r="N79" t="n">
+      <c r="O79" t="n">
         <v>7072080</v>
       </c>
     </row>
@@ -3966,22 +4361,27 @@
       <c r="H80" t="n">
         <v>4.2</v>
       </c>
-      <c r="I80" t="n">
+      <c r="I80" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J80" t="n">
         <v>8086575</v>
       </c>
-      <c r="J80" t="n">
+      <c r="K80" t="n">
         <v>3198862</v>
       </c>
-      <c r="K80" t="n">
+      <c r="L80" t="n">
         <v>646171</v>
       </c>
-      <c r="L80" t="n">
+      <c r="M80" t="n">
         <v>3087942</v>
       </c>
-      <c r="M80" t="n">
+      <c r="N80" t="n">
         <v>7071915</v>
       </c>
-      <c r="N80" t="n">
+      <c r="O80" t="n">
         <v>6750622</v>
       </c>
     </row>
@@ -4010,22 +4410,27 @@
       <c r="H81" t="n">
         <v>4.4</v>
       </c>
-      <c r="I81" t="n">
+      <c r="I81" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J81" t="n">
         <v>8279112</v>
       </c>
-      <c r="J81" t="n">
+      <c r="K81" t="n">
         <v>3046536</v>
       </c>
-      <c r="K81" t="n">
+      <c r="L81" t="n">
         <v>697184</v>
       </c>
-      <c r="L81" t="n">
+      <c r="M81" t="n">
         <v>3144086</v>
       </c>
-      <c r="M81" t="n">
+      <c r="N81" t="n">
         <v>6918178</v>
       </c>
-      <c r="N81" t="n">
+      <c r="O81" t="n">
         <v>7072080</v>
       </c>
     </row>
@@ -4054,22 +4459,27 @@
       <c r="H82" t="n">
         <v>4.4</v>
       </c>
-      <c r="I82" t="n">
+      <c r="I82" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J82" t="n">
         <v>8471650</v>
       </c>
-      <c r="J82" t="n">
+      <c r="K82" t="n">
         <v>3236944</v>
       </c>
-      <c r="K82" t="n">
+      <c r="L82" t="n">
         <v>646171</v>
       </c>
-      <c r="L82" t="n">
+      <c r="M82" t="n">
         <v>3593241</v>
       </c>
-      <c r="M82" t="n">
+      <c r="N82" t="n">
         <v>7225653</v>
       </c>
-      <c r="N82" t="n">
+      <c r="O82" t="n">
         <v>7072080</v>
       </c>
     </row>
@@ -4098,22 +4508,27 @@
       <c r="H83" t="n">
         <v>4.4</v>
       </c>
-      <c r="I83" t="n">
+      <c r="I83" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J83" t="n">
         <v>8471650</v>
       </c>
-      <c r="J83" t="n">
+      <c r="K83" t="n">
         <v>3198862</v>
       </c>
-      <c r="K83" t="n">
+      <c r="L83" t="n">
         <v>578153</v>
       </c>
-      <c r="L83" t="n">
+      <c r="M83" t="n">
         <v>3256375</v>
       </c>
-      <c r="M83" t="n">
+      <c r="N83" t="n">
         <v>7071915</v>
       </c>
-      <c r="N83" t="n">
+      <c r="O83" t="n">
         <v>7072080</v>
       </c>
     </row>
@@ -4142,22 +4557,27 @@
       <c r="H84" t="n">
         <v>4.3</v>
       </c>
-      <c r="I84" t="n">
+      <c r="I84" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J84" t="n">
         <v>8086575</v>
       </c>
-      <c r="J84" t="n">
+      <c r="K84" t="n">
         <v>3084617</v>
       </c>
-      <c r="K84" t="n">
+      <c r="L84" t="n">
         <v>527139</v>
       </c>
-      <c r="L84" t="n">
+      <c r="M84" t="n">
         <v>3256375</v>
       </c>
-      <c r="M84" t="n">
+      <c r="N84" t="n">
         <v>6610703</v>
       </c>
-      <c r="N84" t="n">
+      <c r="O84" t="n">
         <v>6911351</v>
       </c>
     </row>
@@ -4186,22 +4606,27 @@
       <c r="H85" t="n">
         <v>4.3</v>
       </c>
-      <c r="I85" t="n">
+      <c r="I85" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J85" t="n">
         <v>8086575</v>
       </c>
-      <c r="J85" t="n">
+      <c r="K85" t="n">
         <v>3008454</v>
       </c>
-      <c r="K85" t="n">
+      <c r="L85" t="n">
         <v>459121</v>
       </c>
-      <c r="L85" t="n">
+      <c r="M85" t="n">
         <v>3312519</v>
       </c>
-      <c r="M85" t="n">
+      <c r="N85" t="n">
         <v>6764441</v>
       </c>
-      <c r="N85" t="n">
+      <c r="O85" t="n">
         <v>6911351</v>
       </c>
     </row>
@@ -4230,22 +4655,27 @@
       <c r="H86" t="n">
         <v>4.4</v>
       </c>
-      <c r="I86" t="n">
+      <c r="I86" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J86" t="n">
         <v>8078116</v>
       </c>
-      <c r="J86" t="n">
+      <c r="K86" t="n">
         <v>2880600</v>
       </c>
-      <c r="K86" t="n">
+      <c r="L86" t="n">
         <v>653094</v>
       </c>
-      <c r="L86" t="n">
+      <c r="M86" t="n">
         <v>3338514</v>
       </c>
-      <c r="M86" t="n">
+      <c r="N86" t="n">
         <v>6666320</v>
       </c>
-      <c r="N86" t="n">
+      <c r="O86" t="n">
         <v>7127643</v>
       </c>
     </row>
@@ -4274,22 +4704,27 @@
       <c r="H87" t="n">
         <v>4.2</v>
       </c>
-      <c r="I87" t="n">
+      <c r="I87" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J87" t="n">
         <v>7693444</v>
       </c>
-      <c r="J87" t="n">
+      <c r="K87" t="n">
         <v>3034232</v>
       </c>
-      <c r="K87" t="n">
+      <c r="L87" t="n">
         <v>600140</v>
       </c>
-      <c r="L87" t="n">
+      <c r="M87" t="n">
         <v>3165833</v>
       </c>
-      <c r="M87" t="n">
+      <c r="N87" t="n">
         <v>6666320</v>
       </c>
-      <c r="N87" t="n">
+      <c r="O87" t="n">
         <v>6803659</v>
       </c>
     </row>
@@ -4318,22 +4753,27 @@
       <c r="H88" t="n">
         <v>3.9</v>
       </c>
-      <c r="I88" t="n">
+      <c r="I88" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J88" t="n">
         <v>7501107</v>
       </c>
-      <c r="J88" t="n">
+      <c r="K88" t="n">
         <v>3034232</v>
       </c>
-      <c r="K88" t="n">
+      <c r="L88" t="n">
         <v>582489</v>
       </c>
-      <c r="L88" t="n">
+      <c r="M88" t="n">
         <v>2878030</v>
       </c>
-      <c r="M88" t="n">
+      <c r="N88" t="n">
         <v>6511289</v>
       </c>
-      <c r="N88" t="n">
+      <c r="O88" t="n">
         <v>6317684</v>
       </c>
     </row>
@@ -4362,22 +4802,27 @@
       <c r="H89" t="n">
         <v>4.1</v>
       </c>
-      <c r="I89" t="n">
+      <c r="I89" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J89" t="n">
         <v>7501107</v>
       </c>
-      <c r="J89" t="n">
+      <c r="K89" t="n">
         <v>3034232</v>
       </c>
-      <c r="K89" t="n">
+      <c r="L89" t="n">
         <v>582489</v>
       </c>
-      <c r="L89" t="n">
+      <c r="M89" t="n">
         <v>2935590</v>
       </c>
-      <c r="M89" t="n">
+      <c r="N89" t="n">
         <v>6046197</v>
       </c>
-      <c r="N89" t="n">
+      <c r="O89" t="n">
         <v>6641667</v>
       </c>
     </row>
@@ -4406,22 +4851,27 @@
       <c r="H90" t="n">
         <v>4.1</v>
       </c>
-      <c r="I90" t="n">
+      <c r="I90" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J90" t="n">
         <v>7308771</v>
       </c>
-      <c r="J90" t="n">
+      <c r="K90" t="n">
         <v>2957416</v>
       </c>
-      <c r="K90" t="n">
+      <c r="L90" t="n">
         <v>653094</v>
       </c>
-      <c r="L90" t="n">
+      <c r="M90" t="n">
         <v>2993151</v>
       </c>
-      <c r="M90" t="n">
+      <c r="N90" t="n">
         <v>6201228</v>
       </c>
-      <c r="N90" t="n">
+      <c r="O90" t="n">
         <v>6641667</v>
       </c>
     </row>
@@ -4450,22 +4900,27 @@
       <c r="H91" t="n">
         <v>4</v>
       </c>
-      <c r="I91" t="n">
+      <c r="I91" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J91" t="n">
         <v>7308771</v>
       </c>
-      <c r="J91" t="n">
+      <c r="K91" t="n">
         <v>2726967</v>
       </c>
-      <c r="K91" t="n">
+      <c r="L91" t="n">
         <v>635443</v>
       </c>
-      <c r="L91" t="n">
+      <c r="M91" t="n">
         <v>2820469</v>
       </c>
-      <c r="M91" t="n">
+      <c r="N91" t="n">
         <v>6201228</v>
       </c>
-      <c r="N91" t="n">
+      <c r="O91" t="n">
         <v>6479676</v>
       </c>
     </row>
@@ -4494,22 +4949,27 @@
       <c r="H92" t="n">
         <v>3.9</v>
       </c>
-      <c r="I92" t="n">
+      <c r="I92" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J92" t="n">
         <v>7116435</v>
       </c>
-      <c r="J92" t="n">
+      <c r="K92" t="n">
         <v>2842192</v>
       </c>
-      <c r="K92" t="n">
+      <c r="L92" t="n">
         <v>670745</v>
       </c>
-      <c r="L92" t="n">
+      <c r="M92" t="n">
         <v>2935590</v>
       </c>
-      <c r="M92" t="n">
+      <c r="N92" t="n">
         <v>6201228</v>
       </c>
-      <c r="N92" t="n">
+      <c r="O92" t="n">
         <v>6317684</v>
       </c>
     </row>
@@ -4538,22 +4998,27 @@
       <c r="H93" t="n">
         <v>4</v>
       </c>
-      <c r="I93" t="n">
+      <c r="I93" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J93" t="n">
         <v>7308771</v>
       </c>
-      <c r="J93" t="n">
+      <c r="K93" t="n">
         <v>2957416</v>
       </c>
-      <c r="K93" t="n">
+      <c r="L93" t="n">
         <v>688396</v>
       </c>
-      <c r="L93" t="n">
+      <c r="M93" t="n">
         <v>2993151</v>
       </c>
-      <c r="M93" t="n">
+      <c r="N93" t="n">
         <v>6356258</v>
       </c>
-      <c r="N93" t="n">
+      <c r="O93" t="n">
         <v>6479676</v>
       </c>
     </row>
@@ -4582,22 +5047,27 @@
       <c r="H94" t="n">
         <v>3.9</v>
       </c>
-      <c r="I94" t="n">
+      <c r="I94" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J94" t="n">
         <v>7116435</v>
       </c>
-      <c r="J94" t="n">
+      <c r="K94" t="n">
         <v>2765376</v>
       </c>
-      <c r="K94" t="n">
+      <c r="L94" t="n">
         <v>635443</v>
       </c>
-      <c r="L94" t="n">
+      <c r="M94" t="n">
         <v>2935590</v>
       </c>
-      <c r="M94" t="n">
+      <c r="N94" t="n">
         <v>6046197</v>
       </c>
-      <c r="N94" t="n">
+      <c r="O94" t="n">
         <v>6317684</v>
       </c>
     </row>
@@ -4626,22 +5096,27 @@
       <c r="H95" t="n">
         <v>3.700000000000001</v>
       </c>
-      <c r="I95" t="n">
+      <c r="I95" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J95" t="n">
         <v>6731763</v>
       </c>
-      <c r="J95" t="n">
+      <c r="K95" t="n">
         <v>2842192</v>
       </c>
-      <c r="K95" t="n">
+      <c r="L95" t="n">
         <v>529536</v>
       </c>
-      <c r="L95" t="n">
+      <c r="M95" t="n">
         <v>2820469</v>
       </c>
-      <c r="M95" t="n">
+      <c r="N95" t="n">
         <v>5891166</v>
       </c>
-      <c r="N95" t="n">
+      <c r="O95" t="n">
         <v>5993700</v>
       </c>
     </row>
@@ -4670,22 +5145,27 @@
       <c r="H96" t="n">
         <v>3.700000000000001</v>
       </c>
-      <c r="I96" t="n">
+      <c r="I96" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J96" t="n">
         <v>7116435</v>
       </c>
-      <c r="J96" t="n">
+      <c r="K96" t="n">
         <v>2842192</v>
       </c>
-      <c r="K96" t="n">
+      <c r="L96" t="n">
         <v>529536</v>
       </c>
-      <c r="L96" t="n">
+      <c r="M96" t="n">
         <v>2762908</v>
       </c>
-      <c r="M96" t="n">
+      <c r="N96" t="n">
         <v>5891166</v>
       </c>
-      <c r="N96" t="n">
+      <c r="O96" t="n">
         <v>5993700</v>
       </c>
     </row>
@@ -4714,22 +5194,27 @@
       <c r="H97" t="n">
         <v>3.700000000000001</v>
       </c>
-      <c r="I97" t="n">
+      <c r="I97" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J97" t="n">
         <v>7116435</v>
       </c>
-      <c r="J97" t="n">
+      <c r="K97" t="n">
         <v>2573336</v>
       </c>
-      <c r="K97" t="n">
+      <c r="L97" t="n">
         <v>441280</v>
       </c>
-      <c r="L97" t="n">
+      <c r="M97" t="n">
         <v>2878030</v>
       </c>
-      <c r="M97" t="n">
+      <c r="N97" t="n">
         <v>5736135</v>
       </c>
-      <c r="N97" t="n">
+      <c r="O97" t="n">
         <v>5993700</v>
       </c>
     </row>
@@ -4758,22 +5243,27 @@
       <c r="H98" t="n">
         <v>3.600000000000001</v>
       </c>
-      <c r="I98" t="n">
+      <c r="I98" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J98" t="n">
         <v>6724095</v>
       </c>
-      <c r="J98" t="n">
+      <c r="K98" t="n">
         <v>2899177</v>
       </c>
-      <c r="K98" t="n">
+      <c r="L98" t="n">
         <v>535344</v>
       </c>
-      <c r="L98" t="n">
+      <c r="M98" t="n">
         <v>2924180</v>
       </c>
-      <c r="M98" t="n">
+      <c r="N98" t="n">
         <v>5917584</v>
       </c>
-      <c r="N98" t="n">
+      <c r="O98" t="n">
         <v>5859813</v>
       </c>
     </row>
@@ -4802,22 +5292,27 @@
       <c r="H99" t="n">
         <v>3.8</v>
       </c>
-      <c r="I99" t="n">
+      <c r="I99" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J99" t="n">
         <v>7108329</v>
       </c>
-      <c r="J99" t="n">
+      <c r="K99" t="n">
         <v>2589931</v>
       </c>
-      <c r="K99" t="n">
+      <c r="L99" t="n">
         <v>517499</v>
       </c>
-      <c r="L99" t="n">
+      <c r="M99" t="n">
         <v>2865696</v>
       </c>
-      <c r="M99" t="n">
+      <c r="N99" t="n">
         <v>5761858</v>
       </c>
-      <c r="N99" t="n">
+      <c r="O99" t="n">
         <v>6185358</v>
       </c>
     </row>
@@ -4846,22 +5341,27 @@
       <c r="H100" t="n">
         <v>3.700000000000001</v>
       </c>
-      <c r="I100" t="n">
+      <c r="I100" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J100" t="n">
         <v>6916212</v>
       </c>
-      <c r="J100" t="n">
+      <c r="K100" t="n">
         <v>2628587</v>
       </c>
-      <c r="K100" t="n">
+      <c r="L100" t="n">
         <v>553188</v>
       </c>
-      <c r="L100" t="n">
+      <c r="M100" t="n">
         <v>2924180</v>
       </c>
-      <c r="M100" t="n">
+      <c r="N100" t="n">
         <v>5761858</v>
       </c>
-      <c r="N100" t="n">
+      <c r="O100" t="n">
         <v>6022586</v>
       </c>
     </row>
@@ -4890,22 +5390,27 @@
       <c r="H101" t="n">
         <v>3.5</v>
       </c>
-      <c r="I101" t="n">
+      <c r="I101" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J101" t="n">
         <v>6916212</v>
       </c>
-      <c r="J101" t="n">
+      <c r="K101" t="n">
         <v>2473964</v>
       </c>
-      <c r="K101" t="n">
+      <c r="L101" t="n">
         <v>499654</v>
       </c>
-      <c r="L101" t="n">
+      <c r="M101" t="n">
         <v>2807212</v>
       </c>
-      <c r="M101" t="n">
+      <c r="N101" t="n">
         <v>5761858</v>
       </c>
-      <c r="N101" t="n">
+      <c r="O101" t="n">
         <v>5697041</v>
       </c>
     </row>
@@ -4934,22 +5439,27 @@
       <c r="H102" t="n">
         <v>3.4</v>
       </c>
-      <c r="I102" t="n">
+      <c r="I102" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J102" t="n">
         <v>6724095</v>
       </c>
-      <c r="J102" t="n">
+      <c r="K102" t="n">
         <v>2280686</v>
       </c>
-      <c r="K102" t="n">
+      <c r="L102" t="n">
         <v>392585</v>
       </c>
-      <c r="L102" t="n">
+      <c r="M102" t="n">
         <v>2865696</v>
       </c>
-      <c r="M102" t="n">
+      <c r="N102" t="n">
         <v>5606132</v>
       </c>
-      <c r="N102" t="n">
+      <c r="O102" t="n">
         <v>5534268</v>
       </c>
     </row>
@@ -4978,22 +5488,27 @@
       <c r="H103" t="n">
         <v>3.600000000000001</v>
       </c>
-      <c r="I103" t="n">
+      <c r="I103" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J103" t="n">
         <v>6724095</v>
       </c>
-      <c r="J103" t="n">
+      <c r="K103" t="n">
         <v>2512620</v>
       </c>
-      <c r="K103" t="n">
+      <c r="L103" t="n">
         <v>571033</v>
       </c>
-      <c r="L103" t="n">
+      <c r="M103" t="n">
         <v>2631762</v>
       </c>
-      <c r="M103" t="n">
+      <c r="N103" t="n">
         <v>5761858</v>
       </c>
-      <c r="N103" t="n">
+      <c r="O103" t="n">
         <v>5859813</v>
       </c>
     </row>
@@ -5022,22 +5537,27 @@
       <c r="H104" t="n">
         <v>3.600000000000001</v>
       </c>
-      <c r="I104" t="n">
+      <c r="I104" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J104" t="n">
         <v>6339861</v>
       </c>
-      <c r="J104" t="n">
+      <c r="K104" t="n">
         <v>2551276</v>
       </c>
-      <c r="K104" t="n">
+      <c r="L104" t="n">
         <v>553188</v>
       </c>
-      <c r="L104" t="n">
+      <c r="M104" t="n">
         <v>2573278</v>
       </c>
-      <c r="M104" t="n">
+      <c r="N104" t="n">
         <v>5294680</v>
       </c>
-      <c r="N104" t="n">
+      <c r="O104" t="n">
         <v>5859813</v>
       </c>
     </row>
@@ -5066,22 +5586,27 @@
       <c r="H105" t="n">
         <v>3.5</v>
       </c>
-      <c r="I105" t="n">
+      <c r="I105" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J105" t="n">
         <v>6531978</v>
       </c>
-      <c r="J105" t="n">
+      <c r="K105" t="n">
         <v>2435309</v>
       </c>
-      <c r="K105" t="n">
+      <c r="L105" t="n">
         <v>535344</v>
       </c>
-      <c r="L105" t="n">
+      <c r="M105" t="n">
         <v>2748729</v>
       </c>
-      <c r="M105" t="n">
+      <c r="N105" t="n">
         <v>5450406</v>
       </c>
-      <c r="N105" t="n">
+      <c r="O105" t="n">
         <v>5697041</v>
       </c>
     </row>
@@ -5110,22 +5635,27 @@
       <c r="H106" t="n">
         <v>3.3</v>
       </c>
-      <c r="I106" t="n">
+      <c r="I106" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J106" t="n">
         <v>6339861</v>
       </c>
-      <c r="J106" t="n">
+      <c r="K106" t="n">
         <v>2396653</v>
       </c>
-      <c r="K106" t="n">
+      <c r="L106" t="n">
         <v>624568</v>
       </c>
-      <c r="L106" t="n">
+      <c r="M106" t="n">
         <v>2690245</v>
       </c>
-      <c r="M106" t="n">
+      <c r="N106" t="n">
         <v>5294680</v>
       </c>
-      <c r="N106" t="n">
+      <c r="O106" t="n">
         <v>5371495</v>
       </c>
     </row>
@@ -5154,22 +5684,27 @@
       <c r="H107" t="n">
         <v>3.4</v>
       </c>
-      <c r="I107" t="n">
+      <c r="I107" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J107" t="n">
         <v>6339861</v>
       </c>
-      <c r="J107" t="n">
+      <c r="K107" t="n">
         <v>2435309</v>
       </c>
-      <c r="K107" t="n">
+      <c r="L107" t="n">
         <v>553188</v>
       </c>
-      <c r="L107" t="n">
+      <c r="M107" t="n">
         <v>2573278</v>
       </c>
-      <c r="M107" t="n">
+      <c r="N107" t="n">
         <v>5450406</v>
       </c>
-      <c r="N107" t="n">
+      <c r="O107" t="n">
         <v>5534268</v>
       </c>
     </row>
@@ -5198,22 +5733,27 @@
       <c r="H108" t="n">
         <v>3.4</v>
       </c>
-      <c r="I108" t="n">
+      <c r="I108" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J108" t="n">
         <v>6531978</v>
       </c>
-      <c r="J108" t="n">
+      <c r="K108" t="n">
         <v>2357997</v>
       </c>
-      <c r="K108" t="n">
+      <c r="L108" t="n">
         <v>499654</v>
       </c>
-      <c r="L108" t="n">
+      <c r="M108" t="n">
         <v>2631762</v>
       </c>
-      <c r="M108" t="n">
+      <c r="N108" t="n">
         <v>5138954</v>
       </c>
-      <c r="N108" t="n">
+      <c r="O108" t="n">
         <v>5534268</v>
       </c>
     </row>
@@ -5242,22 +5782,27 @@
       <c r="H109" t="n">
         <v>3.5</v>
       </c>
-      <c r="I109" t="n">
+      <c r="I109" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J109" t="n">
         <v>6531978</v>
       </c>
-      <c r="J109" t="n">
+      <c r="K109" t="n">
         <v>2551276</v>
       </c>
-      <c r="K109" t="n">
+      <c r="L109" t="n">
         <v>588878</v>
       </c>
-      <c r="L109" t="n">
+      <c r="M109" t="n">
         <v>2573278</v>
       </c>
-      <c r="M109" t="n">
+      <c r="N109" t="n">
         <v>5606132</v>
       </c>
-      <c r="N109" t="n">
+      <c r="O109" t="n">
         <v>5697041</v>
       </c>
     </row>
@@ -5286,22 +5831,27 @@
       <c r="H110" t="n">
         <v>3.600000000000001</v>
       </c>
-      <c r="I110" t="n">
+      <c r="I110" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J110" t="n">
         <v>6711498</v>
       </c>
-      <c r="J110" t="n">
+      <c r="K110" t="n">
         <v>2643309</v>
       </c>
-      <c r="K110" t="n">
+      <c r="L110" t="n">
         <v>558223</v>
       </c>
-      <c r="L110" t="n">
+      <c r="M110" t="n">
         <v>2836939</v>
       </c>
-      <c r="M110" t="n">
+      <c r="N110" t="n">
         <v>5772000</v>
       </c>
-      <c r="N110" t="n">
+      <c r="O110" t="n">
         <v>5868000</v>
       </c>
     </row>
@@ -5330,22 +5880,27 @@
       <c r="H111" t="n">
         <v>3.4</v>
       </c>
-      <c r="I111" t="n">
+      <c r="I111" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J111" t="n">
         <v>6327984</v>
       </c>
-      <c r="J111" t="n">
+      <c r="K111" t="n">
         <v>2682181</v>
       </c>
-      <c r="K111" t="n">
+      <c r="L111" t="n">
         <v>558223</v>
       </c>
-      <c r="L111" t="n">
+      <c r="M111" t="n">
         <v>2541424</v>
       </c>
-      <c r="M111" t="n">
+      <c r="N111" t="n">
         <v>5460000</v>
       </c>
-      <c r="N111" t="n">
+      <c r="O111" t="n">
         <v>5542000</v>
       </c>
     </row>
@@ -5374,22 +5929,27 @@
       <c r="H112" t="n">
         <v>3.3</v>
       </c>
-      <c r="I112" t="n">
+      <c r="I112" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J112" t="n">
         <v>6519741</v>
       </c>
-      <c r="J112" t="n">
+      <c r="K112" t="n">
         <v>2565565</v>
       </c>
-      <c r="K112" t="n">
+      <c r="L112" t="n">
         <v>558223</v>
       </c>
-      <c r="L112" t="n">
+      <c r="M112" t="n">
         <v>2777836</v>
       </c>
-      <c r="M112" t="n">
+      <c r="N112" t="n">
         <v>5616000</v>
       </c>
-      <c r="N112" t="n">
+      <c r="O112" t="n">
         <v>5379000</v>
       </c>
     </row>
@@ -5418,22 +5978,27 @@
       <c r="H113" t="n">
         <v>3.1</v>
       </c>
-      <c r="I113" t="n">
+      <c r="I113" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J113" t="n">
         <v>5944470</v>
       </c>
-      <c r="J113" t="n">
+      <c r="K113" t="n">
         <v>2565565</v>
       </c>
-      <c r="K113" t="n">
+      <c r="L113" t="n">
         <v>396158</v>
       </c>
-      <c r="L113" t="n">
+      <c r="M113" t="n">
         <v>2482321</v>
       </c>
-      <c r="M113" t="n">
+      <c r="N113" t="n">
         <v>5304000</v>
       </c>
-      <c r="N113" t="n">
+      <c r="O113" t="n">
         <v>5053000</v>
       </c>
     </row>
@@ -5462,22 +6027,27 @@
       <c r="H114" t="n">
         <v>3.3</v>
       </c>
-      <c r="I114" t="n">
+      <c r="I114" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J114" t="n">
         <v>6327984</v>
       </c>
-      <c r="J114" t="n">
+      <c r="K114" t="n">
         <v>2410076</v>
       </c>
-      <c r="K114" t="n">
+      <c r="L114" t="n">
         <v>450180</v>
       </c>
-      <c r="L114" t="n">
+      <c r="M114" t="n">
         <v>2482321</v>
       </c>
-      <c r="M114" t="n">
+      <c r="N114" t="n">
         <v>5304000</v>
       </c>
-      <c r="N114" t="n">
+      <c r="O114" t="n">
         <v>5379000</v>
       </c>
     </row>
@@ -5506,22 +6076,27 @@
       <c r="H115" t="n">
         <v>3.3</v>
       </c>
-      <c r="I115" t="n">
+      <c r="I115" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J115" t="n">
         <v>6327984</v>
       </c>
-      <c r="J115" t="n">
+      <c r="K115" t="n">
         <v>2332332</v>
       </c>
-      <c r="K115" t="n">
+      <c r="L115" t="n">
         <v>378151</v>
       </c>
-      <c r="L115" t="n">
+      <c r="M115" t="n">
         <v>2541424</v>
       </c>
-      <c r="M115" t="n">
+      <c r="N115" t="n">
         <v>5148000</v>
       </c>
-      <c r="N115" t="n">
+      <c r="O115" t="n">
         <v>5379000</v>
       </c>
     </row>
@@ -5550,22 +6125,27 @@
       <c r="H116" t="n">
         <v>3.3</v>
       </c>
-      <c r="I116" t="n">
+      <c r="I116" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J116" t="n">
         <v>6327984</v>
       </c>
-      <c r="J116" t="n">
+      <c r="K116" t="n">
         <v>2293459</v>
       </c>
-      <c r="K116" t="n">
+      <c r="L116" t="n">
         <v>504201</v>
       </c>
-      <c r="L116" t="n">
+      <c r="M116" t="n">
         <v>2659630</v>
       </c>
-      <c r="M116" t="n">
+      <c r="N116" t="n">
         <v>5148000</v>
       </c>
-      <c r="N116" t="n">
+      <c r="O116" t="n">
         <v>5379000</v>
       </c>
     </row>
@@ -5594,22 +6174,27 @@
       <c r="H117" t="n">
         <v>3.3</v>
       </c>
-      <c r="I117" t="n">
+      <c r="I117" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J117" t="n">
         <v>6519741</v>
       </c>
-      <c r="J117" t="n">
+      <c r="K117" t="n">
         <v>2099098</v>
       </c>
-      <c r="K117" t="n">
+      <c r="L117" t="n">
         <v>504201</v>
       </c>
-      <c r="L117" t="n">
+      <c r="M117" t="n">
         <v>2482321</v>
       </c>
-      <c r="M117" t="n">
+      <c r="N117" t="n">
         <v>5148000</v>
       </c>
-      <c r="N117" t="n">
+      <c r="O117" t="n">
         <v>5379000</v>
       </c>
     </row>
@@ -5638,22 +6223,27 @@
       <c r="H118" t="n">
         <v>3.1</v>
       </c>
-      <c r="I118" t="n">
+      <c r="I118" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J118" t="n">
         <v>6136227</v>
       </c>
-      <c r="J118" t="n">
+      <c r="K118" t="n">
         <v>2137971</v>
       </c>
-      <c r="K118" t="n">
+      <c r="L118" t="n">
         <v>450180</v>
       </c>
-      <c r="L118" t="n">
+      <c r="M118" t="n">
         <v>2305013</v>
       </c>
-      <c r="M118" t="n">
+      <c r="N118" t="n">
         <v>4992000</v>
       </c>
-      <c r="N118" t="n">
+      <c r="O118" t="n">
         <v>5053000</v>
       </c>
     </row>
@@ -5682,22 +6272,27 @@
       <c r="H119" t="n">
         <v>3.2</v>
       </c>
-      <c r="I119" t="n">
+      <c r="I119" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J119" t="n">
         <v>6136227</v>
       </c>
-      <c r="J119" t="n">
+      <c r="K119" t="n">
         <v>2137971</v>
       </c>
-      <c r="K119" t="n">
+      <c r="L119" t="n">
         <v>504201</v>
       </c>
-      <c r="L119" t="n">
+      <c r="M119" t="n">
         <v>2423218</v>
       </c>
-      <c r="M119" t="n">
+      <c r="N119" t="n">
         <v>4992000</v>
       </c>
-      <c r="N119" t="n">
+      <c r="O119" t="n">
         <v>5216000</v>
       </c>
     </row>
@@ -5726,22 +6321,27 @@
       <c r="H120" t="n">
         <v>3.2</v>
       </c>
-      <c r="I120" t="n">
+      <c r="I120" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J120" t="n">
         <v>6136227</v>
       </c>
-      <c r="J120" t="n">
+      <c r="K120" t="n">
         <v>2176843</v>
       </c>
-      <c r="K120" t="n">
+      <c r="L120" t="n">
         <v>468187</v>
       </c>
-      <c r="L120" t="n">
+      <c r="M120" t="n">
         <v>2482321</v>
       </c>
-      <c r="M120" t="n">
+      <c r="N120" t="n">
         <v>4992000</v>
       </c>
-      <c r="N120" t="n">
+      <c r="O120" t="n">
         <v>5216000</v>
       </c>
     </row>
@@ -5770,22 +6370,27 @@
       <c r="H121" t="n">
         <v>3.2</v>
       </c>
-      <c r="I121" t="n">
+      <c r="I121" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="J121" t="n">
         <v>6136227</v>
       </c>
-      <c r="J121" t="n">
+      <c r="K121" t="n">
         <v>2293459</v>
       </c>
-      <c r="K121" t="n">
+      <c r="L121" t="n">
         <v>450180</v>
       </c>
-      <c r="L121" t="n">
+      <c r="M121" t="n">
         <v>2482321</v>
       </c>
-      <c r="M121" t="n">
+      <c r="N121" t="n">
         <v>4836000</v>
       </c>
-      <c r="N121" t="n">
+      <c r="O121" t="n">
         <v>5216000</v>
       </c>
     </row>

</xml_diff>